<commit_message>
New dataset + better model
</commit_message>
<xml_diff>
--- a/data/dataset_comments_100_test.xlsx
+++ b/data/dataset_comments_100_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marat.Galiaskarov\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79773\Desktop\ITMO_Competition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FBCE08-1A90-4E31-ADE2-2B2937D17454}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7985382F-2813-44E7-A8BE-D0DEF5E76AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4883" yWindow="0" windowWidth="12465" windowHeight="5535" xr2:uid="{F768725C-C54B-412D-A7AD-C0140B1F9FB8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11280" xr2:uid="{F768725C-C54B-412D-A7AD-C0140B1F9FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>neutral</t>
   </si>
   <si>
-    <t>Class</t>
-  </si>
-  <si>
     <t>16420</t>
   </si>
   <si>
@@ -631,6 +628,9 @@
   </si>
   <si>
     <t>&lt;p class="st0"&gt;Присоединюсь! Огромнейшее спасибо за подарок! Это очень круто! &lt;br&gt;За игрушки на елку отдельное спасибо, нет нет спойлеров не будет :)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>labels</t>
   </si>
 </sst>
 </file>
@@ -675,7 +675,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -710,7 +710,7 @@
     <tableColumn id="1" xr3:uid="{D7EB0DD2-C334-4BC0-A086-3D6A5596CB81}" uniqueName="1" name="UserSenderId" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{0AF74D29-7F98-43AC-AD92-E6287493C3E0}" uniqueName="2" name="SubmitDate" queryTableFieldId="2" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{55EEE53E-ABC1-4C73-9099-EA1346A5504F}" uniqueName="3" name="MessageText" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{3FA6E2BB-F168-40C5-AE2C-401D8F335E11}" uniqueName="4" name="Class" queryTableFieldId="4"/>
+    <tableColumn id="4" xr3:uid="{3FA6E2BB-F168-40C5-AE2C-401D8F335E11}" uniqueName="4" name="labels" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1015,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3DD624-2852-49EE-80DE-525B39D80E91}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1037,18 +1037,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>44188.609100844908</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>44188.593410034722</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>44186.774987928242</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>44176.418639930554</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1">
         <v>44167.688479166667</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1">
         <v>44162.549579629631</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -1126,27 +1126,27 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1">
         <v>44161.416508333336</v>
       </c>
       <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
         <v>56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1">
         <v>44159.709745798609</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1">
         <v>44159.68474394676</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1">
         <v>44159.669966319445</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1">
         <v>44155.680555011575</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="1">
         <v>44155.491415243057</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1210,13 +1210,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="1">
         <v>44152.482950347221</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="1">
         <v>44147.337717442133</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -1238,13 +1238,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="1">
         <v>44145.738685150463</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B17" s="1">
         <v>44145.536398460645</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1">
         <v>44145.507089467596</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" s="1">
         <v>44137.446932789353</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="1">
         <v>44088.523652233795</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -1308,13 +1308,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="1">
         <v>44088.507066863429</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B22" s="1">
         <v>44055.52147349537</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
@@ -1336,13 +1336,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1">
         <v>44047.491192557871</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="1">
         <v>44159.060910532404</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
@@ -1364,13 +1364,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="1">
         <v>44153.655862928237</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1">
         <v>44152.431374108797</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1">
         <v>44151.071190509261</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1">
         <v>44147.731293252313</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
         <v>3</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1">
         <v>44147.383101354164</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
         <v>3</v>
@@ -1434,13 +1434,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" s="1">
         <v>44146.350327858796</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D30" t="s">
         <v>3</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="1">
         <v>44145.724090706019</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
         <v>3</v>
@@ -1462,13 +1462,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" s="1">
         <v>44125.640531828707</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
         <v>3</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B33" s="1">
         <v>44125.554837037038</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D33" t="s">
         <v>3</v>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" s="1">
         <v>44125.473648032406</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" t="s">
         <v>3</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35" s="1">
         <v>44124.436076620368</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
         <v>3</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" s="1">
         <v>44123.282807372685</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" t="s">
         <v>3</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" s="1">
         <v>44077.449806446763</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D37" t="s">
         <v>3</v>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" s="1">
         <v>44074.46823885417</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D38" t="s">
         <v>3</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="1">
         <v>44055.800692395831</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D39" t="s">
         <v>3</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B40" s="1">
         <v>44055.68631099537</v>
       </c>
       <c r="C40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D40" t="s">
         <v>3</v>
@@ -1588,13 +1588,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B41" s="1">
         <v>44054.675259918979</v>
       </c>
       <c r="C41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D41" t="s">
         <v>3</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="1">
         <v>44046.721679710645</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D42" t="s">
         <v>3</v>
@@ -1616,13 +1616,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" s="1">
         <v>44196.527298576388</v>
       </c>
       <c r="C43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -1630,13 +1630,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B44" s="1">
         <v>44196.464265972223</v>
       </c>
       <c r="C44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -1644,13 +1644,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B45" s="1">
         <v>44196.440614733794</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B46" s="1">
         <v>44196.414349803243</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47" s="1">
         <v>44196.411657025463</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B48" s="1">
         <v>44195.830441319442</v>
       </c>
       <c r="C48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -1700,13 +1700,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" s="1">
         <v>44195.72796744213</v>
       </c>
       <c r="C49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
@@ -1714,13 +1714,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B50" s="1">
         <v>44195.726789236112</v>
       </c>
       <c r="C50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B51" s="1">
         <v>44195.700072766202</v>
       </c>
       <c r="C51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" s="1">
         <v>44195.699415740739</v>
       </c>
       <c r="C52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
@@ -1756,13 +1756,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B53" s="1">
         <v>44195.697605821762</v>
       </c>
       <c r="C53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
@@ -1770,13 +1770,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B54" s="1">
         <v>44195.657975381946</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B55" s="1">
         <v>44195.657646793981</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B56" s="1">
         <v>44195.657224733797</v>
       </c>
       <c r="C56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D56" t="s">
         <v>6</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B57" s="1">
         <v>44195.62943429398</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D57" t="s">
         <v>6</v>
@@ -1826,13 +1826,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B58" s="1">
         <v>44195.62034371528</v>
       </c>
       <c r="C58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B59" s="1">
         <v>44195.591959178244</v>
       </c>
       <c r="C59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D59" t="s">
         <v>6</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" s="1">
         <v>44195.561892627316</v>
       </c>
       <c r="C60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D60" t="s">
         <v>6</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B61" s="1">
         <v>44195.517482488423</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
@@ -1882,13 +1882,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B62" s="1">
         <v>44195.440103703702</v>
       </c>
       <c r="C62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D62" t="s">
         <v>6</v>
@@ -1896,13 +1896,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B63" s="1">
         <v>44195.425640972222</v>
       </c>
       <c r="C63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
@@ -1910,13 +1910,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B64" s="1">
         <v>44195.420143553238</v>
       </c>
       <c r="C64" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
@@ -1924,13 +1924,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B65" s="1">
         <v>44195.41551215278</v>
       </c>
       <c r="C65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D65" t="s">
         <v>6</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B66" s="1">
         <v>44195.40600609954</v>
       </c>
       <c r="C66" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D66" t="s">
         <v>6</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B67" s="1">
         <v>44194.706689895836</v>
       </c>
       <c r="C67" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D67" t="s">
         <v>6</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B68" s="1">
         <v>44194.696810995367</v>
       </c>
       <c r="C68" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B69" s="1">
         <v>44194.604168252314</v>
       </c>
       <c r="C69" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D69" t="s">
         <v>6</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B70" s="1">
         <v>44194.497158877311</v>
       </c>
       <c r="C70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D70" t="s">
         <v>6</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B71" s="1">
         <v>44193.545745520831</v>
       </c>
       <c r="C71" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D71" t="s">
         <v>6</v>
@@ -2022,13 +2022,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B72" s="1">
         <v>44193.537803437503</v>
       </c>
       <c r="C72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D72" t="s">
         <v>6</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B73" s="1">
         <v>44193.43054105324</v>
       </c>
       <c r="C73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D73" t="s">
         <v>6</v>
@@ -2050,13 +2050,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B74" s="1">
         <v>44193.413822881943</v>
       </c>
       <c r="C74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D74" t="s">
         <v>6</v>
@@ -2064,13 +2064,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B75" s="1">
         <v>44192.5233409375</v>
       </c>
       <c r="C75" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D75" t="s">
         <v>6</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B76" s="1">
         <v>44191.656473298608</v>
       </c>
       <c r="C76" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D76" t="s">
         <v>6</v>
@@ -2092,13 +2092,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B77" s="1">
         <v>44190.81406084491</v>
       </c>
       <c r="C77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D77" t="s">
         <v>6</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B78" s="1">
         <v>44190.769791979168</v>
       </c>
       <c r="C78" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D78" t="s">
         <v>6</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B79" s="1">
         <v>44190.418613229165</v>
       </c>
       <c r="C79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D79" t="s">
         <v>6</v>
@@ -2134,13 +2134,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B80" s="1">
         <v>44189.767837500003</v>
       </c>
       <c r="C80" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D80" t="s">
         <v>6</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B81" s="1">
         <v>44189.727841701388</v>
       </c>
       <c r="C81" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D81" t="s">
         <v>6</v>
@@ -2162,13 +2162,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B82" s="1">
         <v>44189.727247604169</v>
       </c>
       <c r="C82" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D82" t="s">
         <v>6</v>
@@ -2176,13 +2176,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B83" s="1">
         <v>44189.546201620367</v>
       </c>
       <c r="C83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D83" t="s">
         <v>6</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B84" s="1">
         <v>44189.415405902779</v>
       </c>
       <c r="C84" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D84" t="s">
         <v>6</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B85" s="1">
         <v>44188.785932986109</v>
       </c>
       <c r="C85" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D85" t="s">
         <v>6</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B86" s="1">
         <v>44187.423730590279</v>
       </c>
       <c r="C86" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B87" s="1">
         <v>44187.402491238427</v>
       </c>
       <c r="C87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D87" t="s">
         <v>6</v>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B88" s="1">
         <v>44186.421804201389</v>
       </c>
       <c r="C88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
@@ -2260,13 +2260,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B89" s="1">
         <v>44181.475519444444</v>
       </c>
       <c r="C89" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D89" t="s">
         <v>6</v>
@@ -2274,13 +2274,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B90" s="1">
         <v>44176.548061608795</v>
       </c>
       <c r="C90" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D90" t="s">
         <v>6</v>
@@ -2288,13 +2288,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B91" s="1">
         <v>44176.47964834491</v>
       </c>
       <c r="C91" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B92" s="1">
         <v>44176.43743017361</v>
       </c>
       <c r="C92" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B93" s="1">
         <v>44176.348740393521</v>
       </c>
       <c r="C93" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
@@ -2330,13 +2330,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B94" s="1">
         <v>44168.517939664351</v>
       </c>
       <c r="C94" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B95" s="1">
         <v>44167.743135381941</v>
       </c>
       <c r="C95" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B96" s="1">
         <v>44167.641072569444</v>
       </c>
       <c r="C96" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D96" t="s">
         <v>6</v>
@@ -2372,13 +2372,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B97" s="1">
         <v>44166.520777349535</v>
       </c>
       <c r="C97" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B98" s="1">
         <v>44166.495222025464</v>
       </c>
       <c r="C98" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D98" t="s">
         <v>6</v>
@@ -2400,13 +2400,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B99" s="1">
         <v>44165.687164780094</v>
       </c>
       <c r="C99" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B100" s="1">
         <v>44165.428206828707</v>
       </c>
       <c r="C100" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D100" t="s">
         <v>6</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B101" s="1">
         <v>44162.695390856483</v>
       </c>
       <c r="C101" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D101" t="s">
         <v>6</v>

</xml_diff>